<commit_message>
Fixed typo in option greeks spreadsheet
</commit_message>
<xml_diff>
--- a/option_greeks/option_greeks.xlsx
+++ b/option_greeks/option_greeks.xlsx
@@ -1,12 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\moone\numerical_methods_youtube\option_greeks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF2E444-5F1B-4A60-ADB6-052C75BF82CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -16,9 +35,6 @@
     <t>Call</t>
   </si>
   <si>
-    <t>Putt</t>
-  </si>
-  <si>
     <t>Stock Price (S)</t>
   </si>
   <si>
@@ -47,24 +63,28 @@
   </si>
   <si>
     <t>Imp. Vol</t>
+  </si>
+  <si>
+    <t>Put</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
     </font>
@@ -74,7 +94,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -84,52 +104,67 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -319,135 +354,144 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="5">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
-        <v>100.0</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="5">
+        <v>105</v>
+      </c>
+      <c r="C3" s="6">
+        <f>( LN(B2/B3) + (B4 + B6^2 / 2) * B5) / (B6 * SQRT(B5))</f>
+        <v>-0.49529461409055059</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C3 - B6 * SQRT(B5)</f>
+        <v>-0.58416885184810496</v>
+      </c>
+      <c r="E3" s="6">
+        <f>NORMDIST(C3, 0, 1, TRUE)</f>
+        <v>0.31019608609845817</v>
+      </c>
+      <c r="F3" s="6">
+        <f>B3 * EXP(-B4 * B5) * (NORMDIST(D3, 0, 1, FALSE) / (B2^2 * B6 * SQRT(B5)))</f>
+        <v>3.9706748072218079E-2</v>
+      </c>
+      <c r="G3" s="6">
+        <f>((-B2 * B6 * NORMDIST(C3, 0, 1, FALSE) / (2 * SQRT(B5))) - B4 * B3 * EXP(-B4* B5) * NORMDIST(D3, 0, 1, TRUE)) * 100 / 365</f>
+        <v>-5.3075020041319316</v>
+      </c>
+      <c r="H3" s="6">
+        <f>NORMDIST(-C3, 0, 1, TRUE)</f>
+        <v>0.68980391390154183</v>
+      </c>
+      <c r="I3" s="6">
+        <f>B3 * EXP(-B4 * B5) * (NORMDIST(D3, 0, 1, FALSE) / (B2^2 * B6 * SQRT(B5)))</f>
+        <v>3.9706748072218079E-2</v>
+      </c>
+      <c r="J3" s="7">
+        <f>((-B2 * B6 * NORMDIST(-C3, 0, 1, FALSE) / (2 * SQRT(B5))) - B4 * B3 * EXP(-B4* B5) * NORMDIST(-D3, 0, 1, TRUE)) * 100 / 365</f>
+        <v>-5.4342301159417579</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="5">
-        <v>105.0</v>
-      </c>
-      <c r="C3" s="6">
-        <f>( ln(B2/B3) + (B4 + B6^2 / 2) * B5) / (B6 * sqrt(B5))</f>
-        <v>-0.4952946141</v>
-      </c>
-      <c r="D3" s="1">
-        <f>C3 - B6 * sqrt(B5)</f>
-        <v>-0.5841688518</v>
-      </c>
-      <c r="E3" s="6">
-        <f>normdist(C3, 0, 1, TRUE)</f>
-        <v>0.3101960861</v>
-      </c>
-      <c r="F3" s="6">
-        <f>B3 * exp(-B4 * B5) * (normdist(D3, 0, 1, FALSE) / (B2^2 * B6 * sqrt(B5)))</f>
-        <v>0.03970674807</v>
-      </c>
-      <c r="G3" s="6">
-        <f>((-B2 * B6 * normdist(C3, 0, 1, FALSE) / (2 * sqrt(B5))) - B4 * B3 * exp(-B4* B5) * normdist(D3, 0, 1, True)) * 100 / 365</f>
-        <v>-5.307502004</v>
-      </c>
-      <c r="H3" s="6">
-        <f>normdist(-C3, 0, 1, TRUE)</f>
-        <v>0.6898039139</v>
-      </c>
-      <c r="I3" s="6">
-        <f>B3 * exp(-B4 * B5) * (normdist(D3, 0, 1, FALSE) / (B2^2 * B6 * sqrt(B5)))</f>
-        <v>0.03970674807</v>
-      </c>
-      <c r="J3" s="7">
-        <f>((-B2 * B6 * normdist(-C3, 0, 1, FALSE) / (2 * sqrt(B5))) - B4 * B3 * exp(-B4* B5) * normdist(-D3, 0, 1, True)) * 100 / 365</f>
-        <v>-5.434230116</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="B4" s="5">
         <v>0.01</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8">
         <f>30/365</f>
-        <v>0.08219178082</v>
+        <v>8.2191780821917804E-2</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5">
         <v>0.31</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10">
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
     </row>
@@ -456,6 +500,6 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>